<commit_message>
same version, office machine
</commit_message>
<xml_diff>
--- a/Data/Book1.xlsx
+++ b/Data/Book1.xlsx
@@ -20,7 +20,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
     <sheet name="Sheet3 (2)" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28575,7 +28575,7 @@
   <dimension ref="A1:BQ53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="AG56" sqref="AG56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>

</xml_diff>